<commit_message>
Sprint 1: Create a Server.....Done!!!!!!
Sprint1 Doc updated.
First task for the Project Completed
</commit_message>
<xml_diff>
--- a/Sprint_Docs/Sprint1/FinalSprint1Doc.xlsx
+++ b/Sprint_Docs/Sprint1/FinalSprint1Doc.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="182">
   <si>
     <t>User Stories</t>
   </si>
@@ -710,6 +710,9 @@
   <si>
     <t>Total Hours</t>
   </si>
+  <si>
+    <t>done</t>
+  </si>
 </sst>
 </file>
 
@@ -1157,6 +1160,9 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1175,11 +1181,38 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1198,36 +1231,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1750,11 +1753,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-284082432"/>
-        <c:axId val="-284073728"/>
+        <c:axId val="-1231104752"/>
+        <c:axId val="-1231110736"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-284082432"/>
+        <c:axId val="-1231104752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1792,7 +1795,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-284073728"/>
+        <c:crossAx val="-1231110736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1800,7 +1803,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-284073728"/>
+        <c:axId val="-1231110736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +1855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-284082432"/>
+        <c:crossAx val="-1231104752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4007,20 +4010,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="38"/>
-      <c r="E1" s="47"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="2" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
       <c r="D2" s="38"/>
-      <c r="E2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
@@ -5534,16 +5537,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="52"/>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
     </row>
@@ -5982,21 +5985,21 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="61"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="67"/>
-      <c r="C35" s="68">
+      <c r="B35" s="54"/>
+      <c r="C35" s="55">
         <f>SUM(C4:C34)</f>
         <v>274</v>
       </c>
-      <c r="D35" s="69"/>
+      <c r="D35" s="56"/>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6955,10 +6958,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -13175,7 +13178,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23:P23"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13192,88 +13195,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
     </row>
     <row r="2" spans="1:20" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
     </row>
     <row r="3" spans="1:20" s="31" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="66" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56" t="s">
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56" t="s">
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
     </row>
     <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
       <c r="G4" s="35" t="s">
         <v>21</v>
       </c>
@@ -13439,7 +13442,7 @@
         <v>145</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
@@ -13816,45 +13819,45 @@
       <c r="P21" s="43"/>
     </row>
     <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="B23" s="63">
+      <c r="B23" s="60">
         <f>SUM(B5:B22)</f>
         <v>112</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="65"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="62"/>
     </row>
     <row r="24" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -30346,7 +30349,7 @@
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="N3:P3"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E21">
       <formula1>"to do, parked, in progress, done, blocked, dropped"</formula1>
     </dataValidation>
@@ -30387,38 +30390,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="58" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="58" t="s">
+      <c r="F2" s="59"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="69"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -41540,13 +41543,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Sprint Updates: Create Tables - Done
All the required tables needed as per ER diagram are created on the
MySql server
</commit_message>
<xml_diff>
--- a/Sprint_Docs/Sprint1/FinalSprint1Doc.xlsx
+++ b/Sprint_Docs/Sprint1/FinalSprint1Doc.xlsx
@@ -838,7 +838,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,6 +884,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7AF13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1231,6 +1237,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1753,11 +1762,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1231104752"/>
-        <c:axId val="-1231110736"/>
+        <c:axId val="-2095017392"/>
+        <c:axId val="-2095015216"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1231104752"/>
+        <c:axId val="-2095017392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1795,7 +1804,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1231110736"/>
+        <c:crossAx val="-2095015216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1803,7 +1812,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1231110736"/>
+        <c:axId val="-2095015216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1855,7 +1864,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1231104752"/>
+        <c:crossAx val="-2095017392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13178,7 +13187,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13441,7 +13450,7 @@
       <c r="D9" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="70" t="s">
         <v>181</v>
       </c>
       <c r="F9" s="43"/>
@@ -13801,8 +13810,8 @@
       <c r="D21" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="E21" s="44" t="s">
-        <v>141</v>
+      <c r="E21" s="70" t="s">
+        <v>181</v>
       </c>
       <c r="F21" s="43"/>
       <c r="G21" s="43"/>

</xml_diff>

<commit_message>
update sprint 1 log
</commit_message>
<xml_diff>
--- a/Sprint_Docs/Sprint1/FinalSprint1Doc.xlsx
+++ b/Sprint_Docs/Sprint1/FinalSprint1Doc.xlsx
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="183">
   <si>
     <t>User Stories</t>
   </si>
@@ -708,6 +708,12 @@
   <si>
     <t>Total Hours</t>
   </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
 </sst>
 </file>
 
@@ -827,7 +833,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -873,6 +879,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7AF13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1220,6 +1232,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1705,28 +1720,28 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>147.0</c:v>
+                  <c:v>214.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128.625</c:v>
+                  <c:v>187.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110.25</c:v>
+                  <c:v>160.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91.875</c:v>
+                  <c:v>133.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73.5</c:v>
+                  <c:v>107.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.125</c:v>
+                  <c:v>80.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.75</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.375</c:v>
+                  <c:v>26.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
@@ -1743,11 +1758,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2147318944"/>
-        <c:axId val="-2125429200"/>
+        <c:axId val="2136737104"/>
+        <c:axId val="2136832448"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2147318944"/>
+        <c:axId val="2136737104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,7 +1801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125429200"/>
+        <c:crossAx val="2136832448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1794,7 +1809,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125429200"/>
+        <c:axId val="2136832448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1847,7 +1862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2147318944"/>
+        <c:crossAx val="2136737104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5514,9 +5529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T954"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35:B35"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5579,7 +5594,7 @@
         <v>109</v>
       </c>
       <c r="C5" s="42">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D5" s="42" t="s">
         <v>62</v>
@@ -5607,7 +5622,7 @@
         <v>140</v>
       </c>
       <c r="C7" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>62</v>
@@ -5649,7 +5664,7 @@
         <v>116</v>
       </c>
       <c r="C10" s="42">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D10" s="42" t="s">
         <v>62</v>
@@ -5663,7 +5678,7 @@
         <v>117</v>
       </c>
       <c r="C11" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D11" s="42" t="s">
         <v>62</v>
@@ -5691,7 +5706,7 @@
         <v>136</v>
       </c>
       <c r="C13" s="42">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>62</v>
@@ -5761,7 +5776,7 @@
         <v>124</v>
       </c>
       <c r="C18" s="42">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D18" s="42" t="s">
         <v>137</v>
@@ -5775,7 +5790,7 @@
         <v>125</v>
       </c>
       <c r="C19" s="42">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D19" s="42" t="s">
         <v>65</v>
@@ -5789,7 +5804,7 @@
         <v>169</v>
       </c>
       <c r="C20" s="42">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D20" s="42" t="s">
         <v>65</v>
@@ -5831,7 +5846,7 @@
         <v>128</v>
       </c>
       <c r="C23" s="42">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D23" s="42" t="s">
         <v>65</v>
@@ -5845,7 +5860,7 @@
         <v>129</v>
       </c>
       <c r="C24" s="42">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D24" s="42" t="s">
         <v>65</v>
@@ -5859,7 +5874,7 @@
         <v>130</v>
       </c>
       <c r="C25" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D25" s="42" t="s">
         <v>62</v>
@@ -5887,7 +5902,7 @@
         <v>132</v>
       </c>
       <c r="C27" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D27" s="42" t="s">
         <v>137</v>
@@ -5971,7 +5986,7 @@
         <v>135</v>
       </c>
       <c r="C33" s="42">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D33" s="42" t="s">
         <v>65</v>
@@ -5990,7 +6005,7 @@
       <c r="B35" s="54"/>
       <c r="C35" s="55">
         <f>SUM(C4:C34)</f>
-        <v>274</v>
+        <v>384</v>
       </c>
       <c r="D35" s="56"/>
     </row>
@@ -13169,9 +13184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13344,8 +13359,8 @@
       <c r="D6" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>141</v>
+      <c r="E6" s="70" t="s">
+        <v>181</v>
       </c>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
@@ -13366,7 +13381,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C7" s="42" t="s">
         <v>62</v>
@@ -13405,7 +13420,7 @@
         <v>144</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
@@ -13434,8 +13449,8 @@
       <c r="D9" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>141</v>
+      <c r="E9" s="70" t="s">
+        <v>181</v>
       </c>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
@@ -13456,7 +13471,7 @@
         <v>114</v>
       </c>
       <c r="B10" s="42">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>62</v>
@@ -13516,7 +13531,7 @@
         <v>117</v>
       </c>
       <c r="B12" s="42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>62</v>
@@ -13546,7 +13561,7 @@
         <v>118</v>
       </c>
       <c r="B13" s="42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>62</v>
@@ -13576,7 +13591,7 @@
         <v>136</v>
       </c>
       <c r="B14" s="42">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>62</v>
@@ -13606,7 +13621,7 @@
         <v>119</v>
       </c>
       <c r="B15" s="42">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>62</v>
@@ -13636,7 +13651,7 @@
         <v>120</v>
       </c>
       <c r="B16" s="42">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>62</v>
@@ -13666,7 +13681,7 @@
         <v>121</v>
       </c>
       <c r="B17" s="42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>62</v>
@@ -13696,7 +13711,7 @@
         <v>122</v>
       </c>
       <c r="B18" s="42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" s="42" t="s">
         <v>62</v>
@@ -13726,7 +13741,7 @@
         <v>127</v>
       </c>
       <c r="B19" s="42">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>62</v>
@@ -13756,7 +13771,7 @@
         <v>130</v>
       </c>
       <c r="B20" s="42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>62</v>
@@ -13786,7 +13801,7 @@
         <v>139</v>
       </c>
       <c r="B21" s="43">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C21" s="42" t="s">
         <v>62</v>
@@ -13835,7 +13850,7 @@
       </c>
       <c r="B23" s="60">
         <f>SUM(B5:B22)</f>
-        <v>147</v>
+        <v>214</v>
       </c>
       <c r="C23" s="61"/>
       <c r="D23" s="61"/>
@@ -30342,7 +30357,7 @@
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="N3:P3"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E21">
       <formula1>"to do, parked, in progress, done, blocked, dropped"</formula1>
     </dataValidation>
@@ -30371,8 +30386,8 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView zoomScale="172" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30533,35 +30548,35 @@
       </c>
       <c r="B6" s="27">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((B4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>147</v>
+        <v>214</v>
       </c>
       <c r="C6" s="28">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((C4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>128.625</v>
+        <v>187.25</v>
       </c>
       <c r="D6" s="29">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((D4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>110.25</v>
+        <v>160.5</v>
       </c>
       <c r="E6" s="27">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((E4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>91.875</v>
+        <v>133.75</v>
       </c>
       <c r="F6" s="28">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((F4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>73.5</v>
+        <v>107</v>
       </c>
       <c r="G6" s="29">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((G4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>55.125</v>
+        <v>80.25</v>
       </c>
       <c r="H6" s="27">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((H4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>36.75</v>
+        <v>53.5</v>
       </c>
       <c r="I6" s="28">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((I4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>18.375</v>
+        <v>26.75</v>
       </c>
       <c r="J6" s="29">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((J4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>

</xml_diff>